<commit_message>
RAG fix new files
</commit_message>
<xml_diff>
--- a/files/kb.xlsx
+++ b/files/kb.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\levin\OneDrive\Документы\dev\Python\MalDina\files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{941DE154-E3D7-4355-A5B1-508F78F3179D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B11803AC-C5C9-413B-A826-CD303B3E88BB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{06C4C993-85AB-4544-B2D8-3913DAB2BB78}"/>
   </bookViews>
@@ -39,9 +39,18 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1" uniqueCount="1">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
   <si>
     <t>отказали в  возврате товара</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Здравствуйте. Пожалуйста, свяжитесь с нами в чате поддержки по WhatsApp 7 (962) 559-29-48. Проверим товар, если брак подтвердиться мы сделаем возврат</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Нет заказа </t>
+  </si>
+  <si>
+    <t>Здравствуйте. мы отгружаем товар со своего склада на Вб и их логистика делает доставку. напиши в тех.поддержку самого Вб, мы не можем повлиять на скорость доставки, ни отменить ее не можем. отслеживайте его доставку в своем личном кабинете</t>
   </si>
 </sst>
 </file>
@@ -417,10 +426,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8B9C76FB-0E8B-4191-8625-F60C98342CCE}">
-  <dimension ref="A1:B1"/>
+  <dimension ref="A1:B2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
+      <selection activeCell="A2" sqref="A2:B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -429,9 +438,20 @@
     <col min="2" max="2" width="41.109375" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:2" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" ht="86.4" x14ac:dyDescent="0.3">
+      <c r="A2" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>3</v>
       </c>
     </row>
   </sheetData>

</xml_diff>